<commit_message>
excel structured import wip
</commit_message>
<xml_diff>
--- a/src/test/resources/excelImport/teststudyStructured.xlsx
+++ b/src/test/resources/excelImport/teststudyStructured.xlsx
@@ -404,13 +404,13 @@
   </sheetPr>
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -672,12 +672,12 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -847,12 +847,12 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -933,12 +933,12 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1018,7 +1018,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,16 +1110,16 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>4</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>81</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>84</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>86</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>89</v>
       </c>

</xml_diff>